<commit_message>
상품 등록 DAO, SQL 최신화, Product VO 변경
</commit_message>
<xml_diff>
--- a/docs/프로그램 목록 v0.3.xlsx
+++ b/docs/프로그램 목록 v0.3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="36" windowWidth="16152" windowHeight="9636" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="36" windowWidth="16152" windowHeight="9636" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="공통" sheetId="3" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="상품관리" sheetId="2" r:id="rId3"/>
     <sheet name="주문관리" sheetId="4" r:id="rId4"/>
     <sheet name="장바구니" sheetId="5" r:id="rId5"/>
+    <sheet name="게시판" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -1020,7 +1021,7 @@
   <dimension ref="A2:H23"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -2047,8 +2048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -2642,7 +2643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -2933,4 +2934,19 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>